<commit_message>
zgłoszenie błędu dot. responsywności, uzupełnienie załączników
</commit_message>
<xml_diff>
--- a/zgłoszenia błędów.xlsx
+++ b/zgłoszenia błędów.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="137">
   <si>
     <t>nr ID</t>
   </si>
@@ -280,12 +280,6 @@
   </si>
   <si>
     <t>Bardziej czytelna czcionka.</t>
-  </si>
-  <si>
-    <t>Dodać panel logowania na stronie głównej.</t>
-  </si>
-  <si>
-    <t>Dodać opcję logowania do sklepu na stronie głównej.</t>
   </si>
   <si>
     <t>Ujednolicić interpunkcję w zakładce Regulamin.</t>
@@ -431,25 +425,42 @@
     <t>Po kliknięciu przycisku "Kupuję i płacę" (przy wyborze płatności za pobraniem") zamówienie zostaje złożone, mimo błędnie wypełnionych pól formularza.</t>
   </si>
   <si>
-    <t>Pasek menu na urządzeniach mobilnych.</t>
-  </si>
-  <si>
-    <t>Samsung</t>
-  </si>
-  <si>
-    <t>Prawidłowo wyświetlające się menu.</t>
-  </si>
-  <si>
     <t>Niewidoczne ikony koszyka oraz menu hamburgerowego.</t>
   </si>
   <si>
-    <t>Niewidoczne ikony koszyków oraz menu hamburgerowego na sekcji nawigacji na urządzeniach mobilnych.</t>
-  </si>
-  <si>
     <t>0018</t>
   </si>
   <si>
     <t>Responsywność strony na urządzeniach mobilnych.</t>
+  </si>
+  <si>
+    <t>Niewidoczne ikony koszyków oraz menu hamburgerowego w sekcji nawigacji na urządzeniach mobilnych.</t>
+  </si>
+  <si>
+    <t>Brak panelu logowania na stronie głównej.</t>
+  </si>
+  <si>
+    <t>Sekcja menu na urządzeniach mobilnych.</t>
+  </si>
+  <si>
+    <t>Wyświetlanie banerów w jednej kolumnie.</t>
+  </si>
+  <si>
+    <t>Wyświetlanie banerów u góry strony obok siebie w dwóch kolumnach.</t>
+  </si>
+  <si>
+    <t>Poprawić responsywność strony na urządzeniach mobilnych (dla rozdzielczości poziomej w zakresie 768px - 992px).</t>
+  </si>
+  <si>
+    <t>Dodać opcję logowania do sklepu na stronie głównej na urządzeniach dekstopowych (rozdzielczość powyżej 764px x1024 px).</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy Tab E
+System operacyjny: Android wersja 4.4.4
+Przeglądarka internetowa: Google Chrome wersja 72.0.3626.121</t>
+  </si>
+  <si>
+    <t>Prawidłowo wyświetlające się ikony oraz menu.</t>
   </si>
 </sst>
 </file>
@@ -736,6 +747,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -744,36 +785,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1128,6 +1139,82 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>78050</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1513414</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>2360082</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Obraz 10" descr="017a.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10576717" y="33517417"/>
+          <a:ext cx="1435364" cy="2296582"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>84667</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>84667</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2538676</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>4011082</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Obraz 12" descr="017a.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10583334" y="25061334"/>
+          <a:ext cx="2454009" cy="3926415"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1418,14 +1505,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="5.625" customWidth="1"/>
-    <col min="2" max="2" width="12.125" customWidth="1"/>
+    <col min="2" max="2" width="14.125" customWidth="1"/>
     <col min="3" max="3" width="13.25" customWidth="1"/>
     <col min="4" max="4" width="19.875" customWidth="1"/>
     <col min="5" max="5" width="26.375" customWidth="1"/>
@@ -1438,20 +1525,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="26.25" customHeight="1">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="18"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="28"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" ht="30.75" customHeight="1" thickBot="1">
       <c r="A2" s="3" t="s">
@@ -1666,23 +1753,23 @@
         <v>17</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F8" s="15" t="s">
         <v>52</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I8" s="11"/>
       <c r="J8" s="11" t="s">
@@ -1700,23 +1787,23 @@
         <v>18</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F9" s="15" t="s">
         <v>52</v>
       </c>
       <c r="G9" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" s="11" t="s">
         <v>91</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>93</v>
       </c>
       <c r="I9" s="11"/>
       <c r="J9" s="11" t="s">
@@ -1734,23 +1821,23 @@
         <v>19</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H10" s="11" t="s">
         <v>101</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>103</v>
       </c>
       <c r="I10" s="11"/>
       <c r="J10" s="11" t="s">
@@ -1768,23 +1855,23 @@
         <v>42</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E11" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="G11" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="F11" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>116</v>
-      </c>
       <c r="H11" s="11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I11" s="11"/>
       <c r="J11" s="11" t="s">
@@ -1802,23 +1889,23 @@
         <v>43</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="H12" s="11" t="s">
         <v>119</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>121</v>
       </c>
       <c r="I12" s="11"/>
       <c r="J12" s="11" t="s">
@@ -1836,25 +1923,25 @@
         <v>44</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>33</v>
       </c>
       <c r="D13" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="G13" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="H13" s="11" t="s">
         <v>124</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>126</v>
       </c>
       <c r="I13" s="11"/>
       <c r="J13" s="11" t="s">
@@ -1867,26 +1954,26 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="90">
+    <row r="14" spans="1:12" ht="323.25" customHeight="1">
       <c r="A14" s="10" t="s">
         <v>45</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E14" s="11"/>
-      <c r="F14" s="11" t="s">
-        <v>128</v>
+      <c r="F14" s="15" t="s">
+        <v>135</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="I14" s="11"/>
       <c r="J14" s="11" t="s">
@@ -1904,11 +1991,11 @@
         <v>46</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>69</v>
@@ -1934,23 +2021,21 @@
         <v>47</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>33</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="C16" s="11"/>
       <c r="D16" s="11" t="s">
-        <v>85</v>
+        <v>134</v>
       </c>
       <c r="E16" s="11"/>
       <c r="F16" s="15" t="s">
         <v>52</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I16" s="11"/>
       <c r="J16" s="11" t="s">
@@ -2000,108 +2085,122 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="154.5" customHeight="1">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D18" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E18" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="F18" s="21" t="s">
+      <c r="F18" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="G18" s="20" t="s">
+      <c r="G18" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="H18" s="20" t="s">
+      <c r="H18" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20" t="s">
+      <c r="I18" s="17"/>
+      <c r="J18" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="K18" s="20" t="s">
+      <c r="K18" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="L18" s="22" t="s">
+      <c r="L18" s="19" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="154.5" customHeight="1">
-      <c r="A19" s="19" t="s">
-        <v>105</v>
+    <row r="19" spans="1:12" ht="190.5" customHeight="1">
+      <c r="A19" s="16" t="s">
+        <v>103</v>
       </c>
       <c r="B19" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
       <c r="E19" s="11"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
+      <c r="F19" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>131</v>
+      </c>
       <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="12"/>
+      <c r="J19" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="K19" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="L19" s="12" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="20" spans="1:12" ht="165.75" thickBot="1">
       <c r="A20" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="B20" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="E20" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="C20" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="23" t="s">
+      <c r="F20" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="G20" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="E20" s="23" t="s">
+      <c r="H20" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="F20" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="G20" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="H20" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="I20" s="23"/>
-      <c r="J20" s="23" t="s">
+      <c r="I20" s="20"/>
+      <c r="J20" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="K20" s="23" t="s">
+      <c r="K20" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="L20" s="25" t="s">
+      <c r="L20" s="22" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="15">
-      <c r="A21" s="26"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="27"/>
-      <c r="K21" s="27"/>
-      <c r="L21" s="27"/>
+      <c r="A21" s="23"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="24"/>
     </row>
     <row r="23" spans="1:12">
       <c r="B23" t="s">
@@ -2162,12 +2261,12 @@
     </row>
     <row r="31" spans="1:12">
       <c r="B31" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:12">
       <c r="B32" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
uzupełnienie zgłoszenia dot. responsywności
</commit_message>
<xml_diff>
--- a/zgłoszenia błędów.xlsx
+++ b/zgłoszenia błędów.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="139">
   <si>
     <t>nr ID</t>
   </si>
@@ -443,15 +443,6 @@
     <t>Sekcja menu na urządzeniach mobilnych.</t>
   </si>
   <si>
-    <t>Wyświetlanie banerów w jednej kolumnie.</t>
-  </si>
-  <si>
-    <t>Wyświetlanie banerów u góry strony obok siebie w dwóch kolumnach.</t>
-  </si>
-  <si>
-    <t>Poprawić responsywność strony na urządzeniach mobilnych (dla rozdzielczości poziomej w zakresie 768px - 992px).</t>
-  </si>
-  <si>
     <t>Dodać opcję logowania do sklepu na stronie głównej na urządzeniach dekstopowych (rozdzielczość powyżej 764px x1024 px).</t>
   </si>
   <si>
@@ -461,6 +452,28 @@
   </si>
   <si>
     <t>Prawidłowo wyświetlające się ikony oraz menu.</t>
+  </si>
+  <si>
+    <t>Poprawić responsywność strony na urządzeniach mobilnych (dla rozdzielczości poziomej poniżej 768px oraz w zakresie 768px - 992px).</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy Tab E
+System operacyjny: Android wersja 4.4.4
+Przeglądarka internetowa: Google Chrome wersja 72.0.3626.121
+LG X cam
+System operacyjny: Android 6.0
+Przeglądarka internetowa: Google Chrome wersja 72.0.3626.121</t>
+  </si>
+  <si>
+    <t>1. Dla rodzielczości do 768px: prawidłowe wyświetlanie baneru z funpage'em na Facebooku.
+2. Dla rozdzielczości 768px - 992px: wyświetlanie banerów u góry strony obok siebie w dwóch kolumnach.</t>
+  </si>
+  <si>
+    <t>1. Dla rodzielczości do 768px: puste pole w miejscu banera.
+2. Dla rozdzielczości 768px - 992px: wyświetlanie banerów w jednej kolumnie.</t>
+  </si>
+  <si>
+    <t>użyteczności</t>
   </si>
 </sst>
 </file>
@@ -800,15 +813,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>89733</xdr:colOff>
+      <xdr:colOff>100317</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>58209</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>2600324</xdr:colOff>
+      <xdr:colOff>3167026</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>1628776</xdr:rowOff>
+      <xdr:rowOff>1873250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -825,8 +838,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10424358" y="2457450"/>
-          <a:ext cx="2510591" cy="1485901"/>
+          <a:off x="10598984" y="2375959"/>
+          <a:ext cx="3066709" cy="1815041"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -838,15 +851,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>147872</xdr:colOff>
+      <xdr:colOff>94954</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>84667</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>2571750</xdr:colOff>
+      <xdr:colOff>3132665</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>1809749</xdr:rowOff>
+      <xdr:rowOff>2233353</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -863,8 +876,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10482497" y="4572000"/>
-          <a:ext cx="2423878" cy="1714499"/>
+          <a:off x="10593621" y="4561417"/>
+          <a:ext cx="3037711" cy="2148686"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -882,9 +895,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>2647948</xdr:colOff>
+      <xdr:colOff>3153833</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>2019300</xdr:rowOff>
+      <xdr:rowOff>2395206</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -901,8 +914,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10391774" y="7237913"/>
-          <a:ext cx="2590799" cy="1925137"/>
+          <a:off x="10555816" y="7237913"/>
+          <a:ext cx="3096684" cy="2301043"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -920,9 +933,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>2609849</xdr:colOff>
+      <xdr:colOff>3100916</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>2009773</xdr:rowOff>
+      <xdr:rowOff>2385585</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -939,8 +952,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10372725" y="10042870"/>
-          <a:ext cx="2571749" cy="1968153"/>
+          <a:off x="10536767" y="10042870"/>
+          <a:ext cx="3062816" cy="2343965"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -952,15 +965,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>25993</xdr:colOff>
+      <xdr:colOff>25992</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>2647949</xdr:colOff>
+      <xdr:colOff>3164821</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>1809750</xdr:rowOff>
+      <xdr:rowOff>2159000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -977,8 +990,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10360618" y="14039850"/>
-          <a:ext cx="2621956" cy="1771650"/>
+          <a:off x="10524659" y="35492267"/>
+          <a:ext cx="3138829" cy="2120900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -990,15 +1003,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>31489</xdr:colOff>
+      <xdr:colOff>31488</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>2638425</xdr:colOff>
+      <xdr:colOff>3174999</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>1819274</xdr:rowOff>
+      <xdr:rowOff>2180004</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1015,8 +1028,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10366114" y="13877925"/>
-          <a:ext cx="2606936" cy="1752599"/>
+          <a:off x="10530155" y="33256008"/>
+          <a:ext cx="3143511" cy="2113329"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1034,9 +1047,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>2585835</xdr:colOff>
+      <xdr:colOff>3197995</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>1295400</xdr:rowOff>
+      <xdr:rowOff>1587500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1053,8 +1066,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10363199" y="13886421"/>
-          <a:ext cx="2557261" cy="1220229"/>
+          <a:off x="10527241" y="14256838"/>
+          <a:ext cx="3169421" cy="1512329"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1072,9 +1085,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>2628783</xdr:colOff>
+      <xdr:colOff>3167651</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>1756833</xdr:rowOff>
+      <xdr:rowOff>2106083</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1091,8 +1104,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10388664" y="15800916"/>
-          <a:ext cx="2580036" cy="1672167"/>
+          <a:off x="10547414" y="16171333"/>
+          <a:ext cx="3118904" cy="2021417"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1104,15 +1117,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>45773</xdr:colOff>
+      <xdr:colOff>66939</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>31749</xdr:rowOff>
+      <xdr:rowOff>84665</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>2603500</xdr:colOff>
+      <xdr:colOff>3221176</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>1782453</xdr:rowOff>
+      <xdr:rowOff>2243666</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1129,8 +1142,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10385690" y="17652999"/>
-          <a:ext cx="2557727" cy="1750704"/>
+          <a:off x="10565606" y="18383248"/>
+          <a:ext cx="3154237" cy="2159001"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1142,15 +1155,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>78050</xdr:colOff>
+      <xdr:colOff>1612633</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:rowOff>63499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1513414</xdr:colOff>
+      <xdr:colOff>3167060</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>2360082</xdr:rowOff>
+      <xdr:rowOff>2550582</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1167,8 +1180,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10576717" y="33517417"/>
-          <a:ext cx="1435364" cy="2296582"/>
+          <a:off x="12111300" y="36480749"/>
+          <a:ext cx="1554427" cy="2487083"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1207,6 +1220,44 @@
         <a:xfrm>
           <a:off x="10583334" y="25061334"/>
           <a:ext cx="2454009" cy="3926415"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>84665</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>21171</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1524000</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>2579989</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Obraz 13" descr="017b.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10583332" y="36438421"/>
+          <a:ext cx="1439335" cy="2558818"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1505,8 +1556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1519,7 +1570,7 @@
     <col min="6" max="6" width="18.875" customWidth="1"/>
     <col min="7" max="7" width="20.5" customWidth="1"/>
     <col min="8" max="8" width="19" customWidth="1"/>
-    <col min="9" max="9" width="35.125" customWidth="1"/>
+    <col min="9" max="9" width="42.75" customWidth="1"/>
     <col min="10" max="10" width="10.25" customWidth="1"/>
     <col min="11" max="11" width="10.625" customWidth="1"/>
   </cols>
@@ -1585,7 +1636,9 @@
       <c r="B3" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
@@ -1619,7 +1672,9 @@
       <c r="B4" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="D4" s="11" t="s">
         <v>54</v>
       </c>
@@ -1653,7 +1708,9 @@
       <c r="B5" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="11"/>
+      <c r="C5" s="11" t="s">
+        <v>138</v>
+      </c>
       <c r="D5" s="11" t="s">
         <v>59</v>
       </c>
@@ -1687,7 +1744,9 @@
       <c r="B6" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="11"/>
+      <c r="C6" s="11" t="s">
+        <v>138</v>
+      </c>
       <c r="D6" s="11" t="s">
         <v>65</v>
       </c>
@@ -1714,14 +1773,16 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="165">
+    <row r="7" spans="1:12" ht="194.25" customHeight="1">
       <c r="A7" s="10" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="11"/>
+      <c r="C7" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="D7" s="11" t="s">
         <v>72</v>
       </c>
@@ -1755,7 +1816,9 @@
       <c r="B8" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C8" s="11"/>
+      <c r="C8" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="D8" s="11" t="s">
         <v>87</v>
       </c>
@@ -1789,7 +1852,9 @@
       <c r="B9" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="C9" s="11"/>
+      <c r="C9" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="D9" s="11" t="s">
         <v>90</v>
       </c>
@@ -1816,14 +1881,16 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="150">
+    <row r="10" spans="1:12" ht="174" customHeight="1">
       <c r="A10" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="C10" s="11"/>
+      <c r="C10" s="11" t="s">
+        <v>34</v>
+      </c>
       <c r="D10" s="11" t="s">
         <v>99</v>
       </c>
@@ -1857,7 +1924,9 @@
       <c r="B11" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="C11" s="11"/>
+      <c r="C11" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="D11" s="11" t="s">
         <v>116</v>
       </c>
@@ -1891,7 +1960,9 @@
       <c r="B12" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="C12" s="11"/>
+      <c r="C12" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="D12" s="11" t="s">
         <v>117</v>
       </c>
@@ -1961,16 +2032,18 @@
       <c r="B14" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="C14" s="11"/>
+      <c r="C14" s="11" t="s">
+        <v>34</v>
+      </c>
       <c r="D14" s="11" t="s">
         <v>128</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="15" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H14" s="11" t="s">
         <v>125</v>
@@ -2023,9 +2096,11 @@
       <c r="B16" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="C16" s="11"/>
+      <c r="C16" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="D16" s="11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E16" s="11"/>
       <c r="F16" s="15" t="s">
@@ -2048,7 +2123,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="153" customHeight="1">
+    <row r="17" spans="1:12" ht="178.5" customHeight="1">
       <c r="A17" s="10" t="s">
         <v>48</v>
       </c>
@@ -2084,7 +2159,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="154.5" customHeight="1">
+    <row r="18" spans="1:12" ht="180" customHeight="1">
       <c r="A18" s="16" t="s">
         <v>49</v>
       </c>
@@ -2120,26 +2195,28 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="190.5" customHeight="1">
+    <row r="19" spans="1:12" ht="226.5" customHeight="1">
       <c r="A19" s="16" t="s">
         <v>103</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="C19" s="11"/>
+      <c r="C19" s="11" t="s">
+        <v>34</v>
+      </c>
       <c r="D19" s="11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E19" s="11"/>
       <c r="F19" s="15" t="s">
         <v>135</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="I19" s="11"/>
       <c r="J19" s="11" t="s">

</xml_diff>

<commit_message>
zgłoszenie błędów dot. responsywności i zarządzania kontem
</commit_message>
<xml_diff>
--- a/zgłoszenia błędów.xlsx
+++ b/zgłoszenia błędów.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="141">
   <si>
     <t>nr ID</t>
   </si>
@@ -87,34 +87,13 @@
     <t>Krytyczny</t>
   </si>
   <si>
-    <t>bardzo poważny</t>
-  </si>
-  <si>
-    <t>poważny</t>
-  </si>
-  <si>
     <t>średni</t>
   </si>
   <si>
     <t>trywialny</t>
   </si>
   <si>
-    <t>pilny</t>
-  </si>
-  <si>
-    <t>następne wydanie</t>
-  </si>
-  <si>
-    <t>przy okazji</t>
-  </si>
-  <si>
-    <t>otwarty</t>
-  </si>
-  <si>
     <t>Rodzaj błędu</t>
-  </si>
-  <si>
-    <t>rodzaj</t>
   </si>
   <si>
     <t>improvement</t>
@@ -304,12 +283,6 @@
   </si>
   <si>
     <t>Po przekierowaniu na Facebooka otwiera się pop-up z komunikatem o niedostępności tej funkcji.</t>
-  </si>
-  <si>
-    <t>drawio</t>
-  </si>
-  <si>
-    <t>ximap</t>
   </si>
   <si>
     <t>Panel logowania i rejestracji dostępny na stronie głównej sklepu.</t>
@@ -474,6 +447,42 @@
   </si>
   <si>
     <t>użyteczności</t>
+  </si>
+  <si>
+    <t>0019</t>
+  </si>
+  <si>
+    <t>0020</t>
+  </si>
+  <si>
+    <t>Brak przycisku z menu w pełnej rozdzielczości ekranu.</t>
+  </si>
+  <si>
+    <t>Przy rozdzielczości powyżej 992px brakuje rozwijanego menu hamburgerowego - brakuje opcji logowania i rejestracji nowego użytkownika.</t>
+  </si>
+  <si>
+    <t>Możliwość zalogowania lub rejestracji nowego użytkownika z poziomu stronu głównej sklepu.</t>
+  </si>
+  <si>
+    <t>Brak opcji logowania i rejestracji z poziomu stronu głównej sklepu.</t>
+  </si>
+  <si>
+    <t>Rejestracja nowego konta i zarządzanie nim</t>
+  </si>
+  <si>
+    <t>Problem z rejestracją nowego konta i wprowadzeniem danych oraz hasła dostępowego.</t>
+  </si>
+  <si>
+    <t>1. Na stronie głównej sklepu wybrać opcję zaloguj się.
+2. W sekcji Zarejestruj się, w polu Adres e-mail podać poprawny adres e-mail celem założenia nowego konta. Kliknąć przycisk Zarejestruj się. Nowy użytkownik zostaje natychmiast automatycznie zalogowany.
+3. Kliknąć w link o tytule Szczegóły konta.
+4. Wypełnić poprawnie pola Imię, Nazwisko, adres e-mail oraz pola dotyczące hasła.</t>
+  </si>
+  <si>
+    <t>Możliwość rejestracji nowego konta, wprowadzenie danych właściciela oraz ustawienie hasła dostępowego.</t>
+  </si>
+  <si>
+    <t>Brak możliwości zapisania hasła do nowego konta, co za tym idzie brak możliwości zapisania danych użytkownika.</t>
   </si>
 </sst>
 </file>
@@ -518,7 +527,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -707,6 +716,71 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -751,9 +825,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -772,32 +843,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -858,8 +932,8 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>3132665</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>2233353</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>4503</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -896,8 +970,8 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>3153833</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>2395206</xdr:rowOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>4431</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1554,10 +1628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1566,8 +1640,8 @@
     <col min="2" max="2" width="14.125" customWidth="1"/>
     <col min="3" max="3" width="13.25" customWidth="1"/>
     <col min="4" max="4" width="19.875" customWidth="1"/>
-    <col min="5" max="5" width="26.375" customWidth="1"/>
-    <col min="6" max="6" width="18.875" customWidth="1"/>
+    <col min="5" max="5" width="33.5" customWidth="1"/>
+    <col min="6" max="6" width="23.625" customWidth="1"/>
     <col min="7" max="7" width="20.5" customWidth="1"/>
     <col min="8" max="8" width="19" customWidth="1"/>
     <col min="9" max="9" width="42.75" customWidth="1"/>
@@ -1576,20 +1650,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="26.25" customHeight="1">
-      <c r="A1" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="28"/>
+      <c r="A1" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="27"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" ht="30.75" customHeight="1" thickBot="1">
       <c r="A2" s="3" t="s">
@@ -1599,7 +1673,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>2</v>
@@ -1629,34 +1703,34 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="125.25" customHeight="1">
+    <row r="3" spans="1:12" ht="97.5" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>52</v>
+        <v>30</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="I3" s="7"/>
       <c r="J3" s="7" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>21</v>
@@ -1670,25 +1744,25 @@
         <v>13</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>52</v>
+        <v>46</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>45</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="I4" s="11"/>
       <c r="J4" s="11" t="s">
@@ -1701,73 +1775,73 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="210">
+    <row r="5" spans="1:12" ht="150">
       <c r="A5" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>45</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="I5" s="11"/>
       <c r="J5" s="11" t="s">
         <v>22</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="L5" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="225">
+    <row r="6" spans="1:12" ht="150">
       <c r="A6" s="10" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>52</v>
+        <v>61</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>45</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="I6" s="11"/>
       <c r="J6" s="11" t="s">
         <v>22</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="L6" s="12" t="s">
         <v>11</v>
@@ -1778,101 +1852,101 @@
         <v>16</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>52</v>
+        <v>62</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>45</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="11" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="L7" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="135">
+    <row r="8" spans="1:12" ht="105">
       <c r="A8" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D8" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="E8" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>96</v>
-      </c>
       <c r="H8" s="11" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="I8" s="11"/>
       <c r="J8" s="11" t="s">
         <v>22</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="L8" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="150">
+    <row r="9" spans="1:12" ht="135">
       <c r="A9" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>52</v>
+        <v>100</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>45</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="I9" s="11"/>
       <c r="J9" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K9" s="11" t="s">
         <v>21</v>
@@ -1886,29 +1960,29 @@
         <v>19</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="F10" s="15" t="s">
         <v>102</v>
       </c>
+      <c r="F10" s="14" t="s">
+        <v>93</v>
+      </c>
       <c r="G10" s="11" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="I10" s="11"/>
       <c r="J10" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K10" s="11" t="s">
         <v>21</v>
@@ -1917,73 +1991,73 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="255">
+    <row r="11" spans="1:12" ht="216" customHeight="1">
       <c r="A11" s="10" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>102</v>
+        <v>103</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>93</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="I11" s="11"/>
       <c r="J11" s="11" t="s">
         <v>22</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="L11" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="150">
+    <row r="12" spans="1:12" ht="135">
       <c r="A12" s="10" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>102</v>
+        <v>109</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>93</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="I12" s="11"/>
       <c r="J12" s="11" t="s">
         <v>22</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="L12" s="12" t="s">
         <v>11</v>
@@ -1991,35 +2065,35 @@
     </row>
     <row r="13" spans="1:12" ht="174" customHeight="1">
       <c r="A13" s="10" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>102</v>
+        <v>113</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>93</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="I13" s="11"/>
       <c r="J13" s="11" t="s">
         <v>22</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="L13" s="12" t="s">
         <v>11</v>
@@ -2027,26 +2101,26 @@
     </row>
     <row r="14" spans="1:12" ht="323.25" customHeight="1">
       <c r="A14" s="10" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="E14" s="11"/>
-      <c r="F14" s="15" t="s">
-        <v>132</v>
+      <c r="F14" s="14" t="s">
+        <v>123</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="I14" s="11"/>
       <c r="J14" s="11" t="s">
@@ -2059,65 +2133,65 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="135">
+    <row r="15" spans="1:12" ht="105">
       <c r="A15" s="10" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>52</v>
+        <v>62</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>45</v>
       </c>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
       <c r="J15" s="11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="L15" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="135">
+    <row r="16" spans="1:12" ht="105">
       <c r="A16" s="10" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="E16" s="11"/>
-      <c r="F16" s="15" t="s">
-        <v>52</v>
+      <c r="F16" s="14" t="s">
+        <v>45</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="I16" s="11"/>
       <c r="J16" s="11" t="s">
         <v>20</v>
       </c>
       <c r="K16" s="11" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="L16" s="12" t="s">
         <v>11</v>
@@ -2125,226 +2199,218 @@
     </row>
     <row r="17" spans="1:12" ht="178.5" customHeight="1">
       <c r="A17" s="10" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>78</v>
+        <v>74</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>71</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="I17" s="11"/>
       <c r="J17" s="11" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="K17" s="11" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="L17" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="180" customHeight="1">
-      <c r="A18" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="C18" s="17" t="s">
+      <c r="A18" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="F18" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="G18" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="H18" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="K18" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="L18" s="19" t="s">
+      <c r="K18" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="L18" s="18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="226.5" customHeight="1">
-      <c r="A19" s="16" t="s">
-        <v>103</v>
+    <row r="19" spans="1:12" ht="216" customHeight="1">
+      <c r="A19" s="15" t="s">
+        <v>94</v>
       </c>
       <c r="B19" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="E19" s="11"/>
+      <c r="F19" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="G19" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="C19" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>136</v>
-      </c>
       <c r="H19" s="11" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="I19" s="11"/>
       <c r="J19" s="11" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="L19" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="165.75" thickBot="1">
-      <c r="A20" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="C20" s="20" t="s">
+    <row r="20" spans="1:12" ht="135">
+      <c r="A20" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="G20" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="H20" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="F20" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="G20" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="H20" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="K20" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="L20" s="22" t="s">
+      <c r="K20" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="L20" s="21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15">
-      <c r="A21" s="23"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="24"/>
-      <c r="K21" s="24"/>
-      <c r="L21" s="24"/>
+    <row r="21" spans="1:12" ht="135">
+      <c r="A21" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="E21" s="11"/>
+      <c r="F21" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="K21" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="L21" s="12" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="23" spans="1:12">
-      <c r="B23" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" t="s">
-        <v>9</v>
+    <row r="22" spans="1:12" ht="165.75" thickBot="1">
+      <c r="A22" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="F22" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="G22" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="H22" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="K22" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="L22" s="24" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
-      <c r="B24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="28.5">
-      <c r="B25" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="B26" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
-      <c r="C27" t="s">
-        <v>25</v>
-      </c>
-      <c r="D27" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="C28" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12">
-      <c r="B31" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12">
-      <c r="B32" t="s">
-        <v>93</v>
-      </c>
+    <row r="25" spans="1:12">
+      <c r="C25" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
zgłoszenie błędów dot. responsywności oraz zarządzania kontem
</commit_message>
<xml_diff>
--- a/zgłoszenia błędów.xlsx
+++ b/zgłoszenia błędów.xlsx
@@ -105,9 +105,6 @@
     <t>funkcjonalny</t>
   </si>
   <si>
-    <t>Slider na stronie głównej sklepu wyświetla tylko 2 z 4 zdjęć</t>
-  </si>
-  <si>
     <t>1. Na stronie głównej https://pocztaksiazkowa.pl/ w jej centralnej części znajduje się slider z hiperłączami do podstron.</t>
   </si>
   <si>
@@ -483,6 +480,9 @@
   </si>
   <si>
     <t>Brak możliwości zapisania hasła do nowego konta, co za tym idzie brak możliwości zapisania danych użytkownika.</t>
+  </si>
+  <si>
+    <t>Slider na stronie głównej sklepu wyświetla tylko 2 z 4 zdjęć.</t>
   </si>
 </sst>
 </file>
@@ -861,6 +861,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -869,9 +872,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1630,8 +1630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1650,20 +1650,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="26.25" customHeight="1">
-      <c r="A1" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="27"/>
+      <c r="A1" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="28"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" ht="30.75" customHeight="1" thickBot="1">
       <c r="A2" s="3" t="s">
@@ -1708,29 +1708,29 @@
         <v>12</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>27</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="F3" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G3" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>32</v>
       </c>
       <c r="I3" s="7"/>
       <c r="J3" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>21</v>
@@ -1744,25 +1744,25 @@
         <v>13</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D4" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="G4" s="11" t="s">
+      <c r="H4" s="11" t="s">
         <v>48</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>49</v>
       </c>
       <c r="I4" s="11"/>
       <c r="J4" s="11" t="s">
@@ -1780,32 +1780,32 @@
         <v>14</v>
       </c>
       <c r="B5" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="D5" s="11" t="s">
+      <c r="E5" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="F5" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="G5" s="11" t="s">
+      <c r="H5" s="11" t="s">
         <v>54</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>55</v>
       </c>
       <c r="I5" s="11"/>
       <c r="J5" s="11" t="s">
         <v>22</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L5" s="12" t="s">
         <v>11</v>
@@ -1816,32 +1816,32 @@
         <v>15</v>
       </c>
       <c r="B6" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="D6" s="11" t="s">
+      <c r="E6" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="H6" s="11" t="s">
         <v>58</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>59</v>
       </c>
       <c r="I6" s="11"/>
       <c r="J6" s="11" t="s">
         <v>22</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L6" s="12" t="s">
         <v>11</v>
@@ -1852,32 +1852,32 @@
         <v>16</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E7" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="F7" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7" s="11" t="s">
+      <c r="H7" s="11" t="s">
         <v>63</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>64</v>
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" s="11" t="s">
         <v>33</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>34</v>
       </c>
       <c r="L7" s="12" t="s">
         <v>11</v>
@@ -1888,32 +1888,32 @@
         <v>17</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G8" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="H8" s="11" t="s">
         <v>87</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>88</v>
       </c>
       <c r="I8" s="11"/>
       <c r="J8" s="11" t="s">
         <v>22</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L8" s="12" t="s">
         <v>11</v>
@@ -1924,25 +1924,25 @@
         <v>18</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D9" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="H9" s="11" t="s">
         <v>83</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>84</v>
       </c>
       <c r="I9" s="11"/>
       <c r="J9" s="11" t="s">
@@ -1960,25 +1960,25 @@
         <v>19</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="G10" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="G10" s="11" t="s">
+      <c r="H10" s="11" t="s">
         <v>91</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>92</v>
       </c>
       <c r="I10" s="11"/>
       <c r="J10" s="11" t="s">
@@ -1993,35 +1993,35 @@
     </row>
     <row r="11" spans="1:12" ht="216" customHeight="1">
       <c r="A11" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G11" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="H11" s="11" t="s">
         <v>105</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>106</v>
       </c>
       <c r="I11" s="11"/>
       <c r="J11" s="11" t="s">
         <v>22</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L11" s="12" t="s">
         <v>11</v>
@@ -2029,35 +2029,35 @@
     </row>
     <row r="12" spans="1:12" ht="135">
       <c r="A12" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D12" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="F12" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="H12" s="11" t="s">
         <v>109</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>110</v>
       </c>
       <c r="I12" s="11"/>
       <c r="J12" s="11" t="s">
         <v>22</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L12" s="12" t="s">
         <v>11</v>
@@ -2065,35 +2065,35 @@
     </row>
     <row r="13" spans="1:12" ht="174" customHeight="1">
       <c r="A13" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>26</v>
       </c>
       <c r="D13" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="E13" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="F13" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="G13" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="F13" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="G13" s="11" t="s">
+      <c r="H13" s="11" t="s">
         <v>114</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>115</v>
       </c>
       <c r="I13" s="11"/>
       <c r="J13" s="11" t="s">
         <v>22</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L13" s="12" t="s">
         <v>11</v>
@@ -2101,26 +2101,26 @@
     </row>
     <row r="14" spans="1:12" ht="323.25" customHeight="1">
       <c r="A14" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>27</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="G14" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="G14" s="11" t="s">
-        <v>124</v>
-      </c>
       <c r="H14" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I14" s="11"/>
       <c r="J14" s="11" t="s">
@@ -2135,20 +2135,20 @@
     </row>
     <row r="15" spans="1:12" ht="105">
       <c r="A15" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
@@ -2157,7 +2157,7 @@
         <v>24</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L15" s="12" t="s">
         <v>11</v>
@@ -2165,33 +2165,33 @@
     </row>
     <row r="16" spans="1:12" ht="105">
       <c r="A16" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E16" s="11"/>
       <c r="F16" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G16" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="H16" s="11" t="s">
         <v>85</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>86</v>
       </c>
       <c r="I16" s="11"/>
       <c r="J16" s="11" t="s">
         <v>20</v>
       </c>
       <c r="K16" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L16" s="12" t="s">
         <v>11</v>
@@ -2199,35 +2199,35 @@
     </row>
     <row r="17" spans="1:12" ht="178.5" customHeight="1">
       <c r="A17" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>26</v>
       </c>
       <c r="D17" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="G17" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>76</v>
-      </c>
       <c r="H17" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I17" s="11"/>
       <c r="J17" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="K17" s="11" t="s">
         <v>33</v>
-      </c>
-      <c r="K17" s="11" t="s">
-        <v>34</v>
       </c>
       <c r="L17" s="12" t="s">
         <v>11</v>
@@ -2235,35 +2235,35 @@
     </row>
     <row r="18" spans="1:12" ht="180" customHeight="1">
       <c r="A18" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>26</v>
       </c>
       <c r="D18" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="F18" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="G18" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="F18" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="G18" s="16" t="s">
+      <c r="H18" s="16" t="s">
         <v>69</v>
-      </c>
-      <c r="H18" s="16" t="s">
-        <v>70</v>
       </c>
       <c r="I18" s="16"/>
       <c r="J18" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="K18" s="16" t="s">
         <v>33</v>
-      </c>
-      <c r="K18" s="16" t="s">
-        <v>34</v>
       </c>
       <c r="L18" s="18" t="s">
         <v>11</v>
@@ -2271,33 +2271,33 @@
     </row>
     <row r="19" spans="1:12" ht="216" customHeight="1">
       <c r="A19" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C19" s="11" t="s">
         <v>27</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E19" s="11"/>
       <c r="F19" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="G19" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="H19" s="11" t="s">
         <v>127</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>128</v>
       </c>
       <c r="I19" s="11"/>
       <c r="J19" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="K19" s="11" t="s">
         <v>33</v>
-      </c>
-      <c r="K19" s="11" t="s">
-        <v>34</v>
       </c>
       <c r="L19" s="12" t="s">
         <v>11</v>
@@ -2305,35 +2305,35 @@
     </row>
     <row r="20" spans="1:12" ht="135">
       <c r="A20" s="15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C20" s="19" t="s">
         <v>26</v>
       </c>
       <c r="D20" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="E20" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="F20" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="G20" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="F20" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="G20" s="19" t="s">
+      <c r="H20" s="19" t="s">
         <v>98</v>
-      </c>
-      <c r="H20" s="19" t="s">
-        <v>99</v>
       </c>
       <c r="I20" s="19"/>
       <c r="J20" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="K20" s="19" t="s">
         <v>33</v>
-      </c>
-      <c r="K20" s="19" t="s">
-        <v>34</v>
       </c>
       <c r="L20" s="21" t="s">
         <v>11</v>
@@ -2341,33 +2341,33 @@
     </row>
     <row r="21" spans="1:12" ht="135">
       <c r="A21" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E21" s="11"/>
       <c r="F21" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G21" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="H21" s="11" t="s">
         <v>134</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>135</v>
       </c>
       <c r="I21" s="11"/>
       <c r="J21" s="11" t="s">
         <v>22</v>
       </c>
       <c r="K21" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L21" s="12" t="s">
         <v>11</v>
@@ -2375,35 +2375,35 @@
     </row>
     <row r="22" spans="1:12" ht="165.75" thickBot="1">
       <c r="A22" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C22" s="23" t="s">
         <v>28</v>
       </c>
       <c r="D22" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="E22" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="E22" s="23" t="s">
+      <c r="F22" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="G22" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="F22" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="G22" s="23" t="s">
+      <c r="H22" s="23" t="s">
         <v>139</v>
-      </c>
-      <c r="H22" s="23" t="s">
-        <v>140</v>
       </c>
       <c r="I22" s="23"/>
       <c r="J22" s="23" t="s">
         <v>22</v>
       </c>
       <c r="K22" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L22" s="24" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
dodanie zgłoszenia o braku liczby egzemplarzy produktu w koszyku
</commit_message>
<xml_diff>
--- a/zgłoszenia błędów.xlsx
+++ b/zgłoszenia błędów.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="149">
   <si>
     <t>nr ID</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>funkcjonalny</t>
+  </si>
+  <si>
+    <t>Slider na stronie głównej sklepu wyświetla tylko 2 z 4 zdjęć</t>
   </si>
   <si>
     <t>1. Na stronie głównej https://pocztaksiazkowa.pl/ w jej centralnej części znajduje się slider z hiperłączami do podstron.</t>
@@ -482,7 +485,30 @@
     <t>Brak możliwości zapisania hasła do nowego konta, co za tym idzie brak możliwości zapisania danych użytkownika.</t>
   </si>
   <si>
-    <t>Slider na stronie głównej sklepu wyświetla tylko 2 z 4 zdjęć.</t>
+    <t>0021</t>
+  </si>
+  <si>
+    <t>System nie wyświetla liczby egzemplarzy tego samego produktu, które chcemy dodoać do koszyka oraz później w samym koszyku.</t>
+  </si>
+  <si>
+    <t>1. Na stronie głównej sklepu wybierz dowolny produkt.
+2. Wejdź na podstronę produktu. W miejscu wyboru ilości egzemplarzy kliknij dowolną ilość razy.
+3. Dodaj produkt do koszyka.</t>
+  </si>
+  <si>
+    <t>System dokladnie pokazuje ile egzemplarzy danego produktu chcemy dodać do koszyka oraz ile dokładnie mamy produktów w koszyku.</t>
+  </si>
+  <si>
+    <t>Brak informacji o ilości produktów jednego typu w koszyku.</t>
+  </si>
+  <si>
+    <t>0022</t>
+  </si>
+  <si>
+    <t>0023</t>
+  </si>
+  <si>
+    <t>Ilość produktów do dodania oraz w koszyku</t>
   </si>
 </sst>
 </file>
@@ -527,7 +553,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -781,6 +807,17 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -792,9 +829,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -861,9 +895,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -872,6 +903,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1332,6 +1369,82 @@
         <a:xfrm>
           <a:off x="10583332" y="36438421"/>
           <a:ext cx="1439335" cy="2558818"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>104426</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>3196167</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>1340955</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Obraz 14" descr="021.JPG"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11430000" y="42035593"/>
+          <a:ext cx="3164417" cy="1236529"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>63499</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>1582127</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>3202133</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>2995083</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Obraz 17" descr="021a.JPG"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11461749" y="43502710"/>
+          <a:ext cx="3138634" cy="1412956"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1630,8 +1743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1650,767 +1763,836 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="26.25" customHeight="1">
-      <c r="A1" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="28"/>
+      <c r="A1" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="26"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="97.5" customHeight="1">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="7" t="s">
+      <c r="B3" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="E3" s="7" t="s">
+      <c r="D3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="F3" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7" t="s">
+      <c r="H3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="I3" s="6"/>
+      <c r="J3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="L3" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="170.25" customHeight="1">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11" t="s">
+      <c r="I4" s="10"/>
+      <c r="J4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="L4" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="150">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="D5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="C5" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="F5" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11" t="s">
+      <c r="H5" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K5" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="L5" s="12" t="s">
+      <c r="K5" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="L5" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="150">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="L6" s="12" t="s">
+      <c r="L6" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="194.25" customHeight="1">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" s="11" t="s">
+      <c r="B7" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="K7" s="11" t="s">
+      <c r="I7" s="10"/>
+      <c r="J7" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="L7" s="12" t="s">
+      <c r="K7" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="105">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="C8" s="11" t="s">
+      <c r="B8" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="H8" s="11" t="s">
+      <c r="D8" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11" t="s">
+      <c r="H8" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K8" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="L8" s="12" t="s">
+      <c r="K8" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="L8" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="135">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="C9" s="11" t="s">
+      <c r="B9" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="E9" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11" t="s">
+      <c r="H9" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="K9" s="11" t="s">
+      <c r="K9" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="L9" s="12" t="s">
+      <c r="L9" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="174" customHeight="1">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="C10" s="11" t="s">
+      <c r="B10" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="F10" s="14" t="s">
+      <c r="D10" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="H10" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="G10" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11" t="s">
+      <c r="I10" s="10"/>
+      <c r="J10" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="K10" s="11" t="s">
+      <c r="K10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="L10" s="12" t="s">
+      <c r="L10" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="216" customHeight="1">
-      <c r="A11" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="11" t="s">
+      <c r="A11" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E11" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="11" t="s">
+      <c r="F11" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H11" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E11" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11" t="s">
+      <c r="I11" s="10"/>
+      <c r="J11" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K11" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="L11" s="12" t="s">
+      <c r="K11" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="L11" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="135">
-      <c r="A12" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="C12" s="11" t="s">
+      <c r="A12" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="E12" s="11" t="s">
+      <c r="D12" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="F12" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="H12" s="11" t="s">
+      <c r="E12" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11" t="s">
+      <c r="F12" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K12" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="L12" s="12" t="s">
+      <c r="K12" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="L12" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="174" customHeight="1">
-      <c r="A13" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="C13" s="11" t="s">
+      <c r="A13" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="E13" s="11" t="s">
+      <c r="D13" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="F13" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="G13" s="11" t="s">
+      <c r="E13" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="F13" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11" t="s">
+      <c r="H13" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K13" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="L13" s="12" t="s">
+      <c r="K13" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="L13" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="323.25" customHeight="1">
-      <c r="A14" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="C14" s="11" t="s">
+      <c r="A14" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="G14" s="11" t="s">
+      <c r="D14" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="H14" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11" t="s">
+      <c r="G14" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K14" s="11" t="s">
+      <c r="K14" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="L14" s="12" t="s">
+      <c r="L14" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="105">
-      <c r="A15" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11" t="s">
+      <c r="A15" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="K15" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="L15" s="12" t="s">
+      <c r="K15" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="L15" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="105">
-      <c r="A16" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="C16" s="11" t="s">
+      <c r="A16" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="H16" s="11" t="s">
+      <c r="D16" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11" t="s">
+      <c r="H16" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K16" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="L16" s="12" t="s">
+      <c r="K16" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="L16" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="178.5" customHeight="1">
-      <c r="A17" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="11" t="s">
+      <c r="A17" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="E17" s="11" t="s">
+      <c r="G17" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="H17" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="F17" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="K17" s="11" t="s">
+      <c r="I17" s="10"/>
+      <c r="J17" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="L17" s="12" t="s">
+      <c r="K17" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="L17" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="180" customHeight="1">
-      <c r="A18" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" s="16" t="s">
+      <c r="A18" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="E18" s="16" t="s">
+      <c r="D18" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="F18" s="17" t="s">
+      <c r="E18" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="H18" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="G18" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="H18" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="K18" s="16" t="s">
+      <c r="I18" s="15"/>
+      <c r="J18" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="L18" s="18" t="s">
+      <c r="K18" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="L18" s="17" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="216" customHeight="1">
-      <c r="A19" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="C19" s="11" t="s">
+      <c r="A19" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="14" t="s">
+      <c r="D19" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="E19" s="10"/>
+      <c r="F19" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="H19" s="11" t="s">
+      <c r="G19" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="K19" s="11" t="s">
+      <c r="H19" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="L19" s="12" t="s">
+      <c r="K19" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="L19" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="135">
-      <c r="A20" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="C20" s="19" t="s">
+      <c r="A20" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="E20" s="19" t="s">
+      <c r="D20" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="F20" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="G20" s="19" t="s">
+      <c r="E20" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="H20" s="19" t="s">
+      <c r="F20" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="G20" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="K20" s="19" t="s">
+      <c r="H20" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="L20" s="21" t="s">
+      <c r="K20" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="L20" s="20" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="135">
-      <c r="A21" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="B21" s="11" t="s">
+      <c r="A21" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="F21" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K21" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="L21" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="165">
+      <c r="A22" s="27" t="s">
         <v>131</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="B22" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C22" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E21" s="11"/>
-      <c r="F21" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11" t="s">
+      <c r="D22" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="K21" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="L21" s="12" t="s">
+      <c r="K22" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="L22" s="17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="165.75" thickBot="1">
-      <c r="A22" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="B22" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="C22" s="23" t="s">
+    <row r="23" spans="1:12" ht="249.75" customHeight="1">
+      <c r="A23" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="C23" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="E22" s="23" t="s">
-        <v>137</v>
-      </c>
-      <c r="F22" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="G22" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="H22" s="23" t="s">
-        <v>139</v>
-      </c>
-      <c r="I22" s="23"/>
-      <c r="J22" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="K22" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="L22" s="24" t="s">
+      <c r="D23" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K23" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="L23" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
-      <c r="C25" s="2"/>
+    <row r="24" spans="1:12" ht="15">
+      <c r="A24" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A25" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="23" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
usunięcie błędu dot. rejestracji nowego konta i administrowania nim
</commit_message>
<xml_diff>
--- a/zgłoszenia błędów.xlsx
+++ b/zgłoszenia błędów.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="144">
   <si>
     <t>nr ID</t>
   </si>
@@ -465,24 +465,6 @@
   </si>
   <si>
     <t>Brak opcji logowania i rejestracji z poziomu stronu głównej sklepu.</t>
-  </si>
-  <si>
-    <t>Rejestracja nowego konta i zarządzanie nim</t>
-  </si>
-  <si>
-    <t>Problem z rejestracją nowego konta i wprowadzeniem danych oraz hasła dostępowego.</t>
-  </si>
-  <si>
-    <t>1. Na stronie głównej sklepu wybrać opcję zaloguj się.
-2. W sekcji Zarejestruj się, w polu Adres e-mail podać poprawny adres e-mail celem założenia nowego konta. Kliknąć przycisk Zarejestruj się. Nowy użytkownik zostaje natychmiast automatycznie zalogowany.
-3. Kliknąć w link o tytule Szczegóły konta.
-4. Wypełnić poprawnie pola Imię, Nazwisko, adres e-mail oraz pola dotyczące hasła.</t>
-  </si>
-  <si>
-    <t>Możliwość rejestracji nowego konta, wprowadzenie danych właściciela oraz ustawienie hasła dostępowego.</t>
-  </si>
-  <si>
-    <t>Brak możliwości zapisania hasła do nowego konta, co za tym idzie brak możliwości zapisania danych użytkownika.</t>
   </si>
   <si>
     <t>0021</t>
@@ -895,6 +877,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -903,12 +891,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1381,18 +1363,18 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>31750</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>104426</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>3196167</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>1340955</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Obraz 14" descr="021.JPG"/>
+        <xdr:cNvPr id="16" name="Obraz 15" descr="021.JPG"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1405,7 +1387,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11430000" y="42035593"/>
+          <a:off x="11430000" y="42025009"/>
           <a:ext cx="3164417" cy="1236529"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1419,18 +1401,18 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>63499</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>1582127</xdr:rowOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>1582126</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>3202133</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>2995083</xdr:rowOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>2592917</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="Obraz 17" descr="021a.JPG"/>
+        <xdr:cNvPr id="17" name="Obraz 16" descr="021a.JPG"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1443,8 +1425,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11461749" y="43502710"/>
-          <a:ext cx="3138634" cy="1412956"/>
+          <a:off x="11461749" y="41407209"/>
+          <a:ext cx="3138634" cy="1010791"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1744,7 +1726,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1763,20 +1745,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="26.25" customHeight="1">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="26"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="28"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" ht="30.75" customHeight="1" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -2486,81 +2468,61 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="165">
-      <c r="A22" s="27" t="s">
+    <row r="22" spans="1:12" ht="216.75" customHeight="1">
+      <c r="A22" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K22" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="L22" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="19.5" customHeight="1">
+      <c r="A23" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="C22" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="F22" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="G22" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="H22" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="K22" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="L22" s="17" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="249.75" customHeight="1">
-      <c r="A23" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="F23" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="H23" s="10" t="s">
-        <v>145</v>
-      </c>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
       <c r="I23" s="10"/>
-      <c r="J23" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="K23" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="L23" s="11" t="s">
-        <v>11</v>
-      </c>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="11"/>
     </row>
     <row r="24" spans="1:12" ht="15">
       <c r="A24" s="9" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
@@ -2578,13 +2540,13 @@
     </row>
     <row r="25" spans="1:12" ht="15.75" thickBot="1">
       <c r="A25" s="21" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B25" s="22"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
-      <c r="F25" s="28"/>
+      <c r="F25" s="25"/>
       <c r="G25" s="22"/>
       <c r="H25" s="22"/>
       <c r="I25" s="22"/>

</xml_diff>